<commit_message>
reconstruction bdd avec page edition
</commit_message>
<xml_diff>
--- a/public/DonneesKm2.xlsx
+++ b/public/DonneesKm2.xlsx
@@ -1019,223 +1019,220 @@
     </row>
     <row r="2" spans="1:109">
       <c r="A2">
-        <v>107656</v>
+        <v>114953</v>
       </c>
       <c r="B2">
-        <v>19373</v>
+        <v>22825</v>
       </c>
       <c r="C2">
-        <v>15905</v>
+        <v>19330</v>
       </c>
       <c r="D2">
-        <v>91133</v>
+        <v>99355</v>
       </c>
       <c r="E2">
-        <v>21348</v>
+        <v>24546</v>
       </c>
       <c r="J2">
-        <v>54994</v>
+        <v>59041</v>
       </c>
       <c r="K2">
-        <v>71778</v>
+        <v>75250</v>
       </c>
       <c r="L2">
-        <v>15257</v>
+        <v>17408</v>
       </c>
       <c r="M2">
-        <v>100336</v>
+        <v>105144</v>
       </c>
       <c r="P2">
-        <v>106894</v>
+        <v>107401</v>
       </c>
       <c r="S2">
-        <v>12800</v>
+        <v>14770</v>
       </c>
       <c r="T2">
-        <v>86026</v>
+        <v>90649</v>
       </c>
       <c r="V2">
-        <v>303320</v>
+        <v>311343</v>
       </c>
       <c r="W2">
-        <v>17528</v>
+        <v>19914</v>
       </c>
       <c r="Z2">
-        <v>45903</v>
+        <v>51079</v>
       </c>
       <c r="AA2">
-        <v>56681</v>
+        <v>62734</v>
       </c>
       <c r="AC2">
-        <v>52408</v>
+        <v>57215</v>
       </c>
       <c r="AD2">
-        <v>182423</v>
+        <v>190793</v>
       </c>
       <c r="AE2">
-        <v>71020</v>
+        <v>72022</v>
       </c>
       <c r="AF2">
-        <v>74982</v>
+        <v>84524</v>
       </c>
       <c r="AG2">
-        <v>52359</v>
+        <v>54576</v>
       </c>
       <c r="AH2">
-        <v>50772</v>
+        <v>54712</v>
       </c>
       <c r="AI2">
-        <v>80475</v>
+        <v>83137</v>
       </c>
       <c r="AJ2">
-        <v>24820</v>
+        <v>27943</v>
       </c>
       <c r="AK2">
-        <v>44570</v>
+        <v>46099</v>
       </c>
       <c r="AL2">
-        <v>259335</v>
+        <v>265414</v>
       </c>
       <c r="AP2">
-        <v>222782</v>
+        <v>228532</v>
       </c>
       <c r="AQ2">
-        <v>15913</v>
+        <v>19242</v>
       </c>
       <c r="AR2">
-        <v>563504</v>
+        <v>578330</v>
       </c>
       <c r="AT2">
-        <v>509053</v>
+        <v>521829</v>
       </c>
       <c r="AU2">
-        <v>10740</v>
+        <v>13085</v>
       </c>
       <c r="AW2">
-        <v>13620</v>
+        <v>16327</v>
       </c>
       <c r="AX2">
-        <v>26976</v>
+        <v>28783</v>
       </c>
       <c r="AY2">
-        <v>87972</v>
+        <v>93448</v>
       </c>
       <c r="AZ2">
-        <v>51102</v>
-      </c>
-      <c r="BC2">
-        <v>24692</v>
+        <v>58382</v>
       </c>
       <c r="BD2">
-        <v>38367</v>
+        <v>42817</v>
       </c>
       <c r="BE2">
-        <v>196227</v>
+        <v>214506</v>
       </c>
       <c r="BF2">
-        <v>200138</v>
+        <v>217250</v>
       </c>
       <c r="BG2">
-        <v>51552</v>
+        <v>55385</v>
       </c>
       <c r="BH2">
-        <v>25142</v>
+        <v>27839</v>
       </c>
       <c r="BI2">
-        <v>99749</v>
+        <v>104840</v>
       </c>
       <c r="BK2">
-        <v>47636</v>
+        <v>53300</v>
       </c>
       <c r="BL2">
-        <v>15924</v>
+        <v>18173</v>
       </c>
       <c r="BO2">
-        <v>136785</v>
+        <v>138632</v>
       </c>
       <c r="BP2">
-        <v>177294</v>
+        <v>179069</v>
       </c>
       <c r="BQ2">
-        <v>49917</v>
+        <v>54860</v>
       </c>
       <c r="BR2">
-        <v>50384</v>
+        <v>54249</v>
       </c>
       <c r="BS2">
-        <v>70875</v>
+        <v>75079</v>
       </c>
       <c r="BT2">
-        <v>20781</v>
+        <v>24324</v>
       </c>
       <c r="BU2">
-        <v>51827</v>
+        <v>57702</v>
       </c>
       <c r="BV2">
-        <v>111618</v>
+        <v>113788</v>
       </c>
       <c r="BZ2">
-        <v>21909</v>
+        <v>24807</v>
       </c>
       <c r="CE2">
-        <v>19147</v>
+        <v>22399</v>
       </c>
       <c r="CG2">
-        <v>66927</v>
+        <v>72883</v>
       </c>
       <c r="CH2">
-        <v>17015</v>
+        <v>19794</v>
       </c>
       <c r="CI2">
-        <v>114925</v>
+        <v>115591</v>
       </c>
       <c r="CJ2">
-        <v>127678</v>
+        <v>128787</v>
       </c>
       <c r="CK2">
-        <v>135520</v>
+        <v>136464</v>
       </c>
       <c r="CL2">
-        <v>18301</v>
+        <v>20509</v>
       </c>
       <c r="CM2">
-        <v>21916</v>
+        <v>24542</v>
       </c>
       <c r="CN2">
-        <v>134720</v>
+        <v>136528</v>
       </c>
       <c r="CQ2">
-        <v>92518</v>
+        <v>93679</v>
       </c>
       <c r="CR2">
-        <v>124007</v>
+        <v>125623</v>
       </c>
       <c r="CS2">
-        <v>82541</v>
+        <v>84677</v>
       </c>
       <c r="CT2">
-        <v>24765</v>
+        <v>27442</v>
       </c>
       <c r="CU2">
-        <v>134015</v>
+        <v>137889</v>
       </c>
       <c r="CV2">
-        <v>196245</v>
+        <v>199897</v>
       </c>
       <c r="CW2">
-        <v>135393</v>
+        <v>138701</v>
       </c>
       <c r="CX2">
-        <v>140945</v>
+        <v>142391</v>
       </c>
       <c r="DB2">
-        <v>50439</v>
+        <v>54680</v>
       </c>
       <c r="DC2">
-        <v>61173</v>
+        <v>62957</v>
       </c>
       <c r="DE2">
-        <v>20777</v>
+        <v>46387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>